<commit_message>
Simplify character asset list and animation state machine.
</commit_message>
<xml_diff>
--- a/Design/Asset List.xlsx
+++ b/Design/Asset List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259F9521-503A-4629-85EE-77ABC72110BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32328A3-31D4-4046-85B1-3AEC2E0146DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
   <si>
     <t>Type</t>
   </si>
@@ -50,15 +50,9 @@
     <t>Idle</t>
   </si>
   <si>
-    <t>Startup</t>
-  </si>
-  <si>
     <t>Throwing</t>
   </si>
   <si>
-    <t>Recorvery</t>
-  </si>
-  <si>
     <t>Teleport</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>Animation Sprites</t>
   </si>
   <si>
-    <t>Teleport_Recovery</t>
-  </si>
-  <si>
     <t>Boomerang</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>Building</t>
   </si>
   <si>
-    <t>_0X(Variants)</t>
-  </si>
-  <si>
     <t>FlyingCar</t>
   </si>
   <si>
@@ -146,84 +134,9 @@
     <t>NJ_</t>
   </si>
   <si>
-    <t>忍者抬起手里剑准备瞄准，一次性过渡动画</t>
-  </si>
-  <si>
-    <t>Catch</t>
-  </si>
-  <si>
-    <t>Empty-handed</t>
-  </si>
-  <si>
-    <t>忍者空手自然站立，循环动画</t>
-  </si>
-  <si>
-    <t>忍者在空手状态下接住飞回来的回旋镖，一次性过渡动画</t>
-  </si>
-  <si>
-    <t>忍者发动传送动作，一次性过渡动画</t>
-  </si>
-  <si>
-    <t>忍者在扔完手里剑后恢复动作到空手站立状态，一次性过渡动画</t>
-  </si>
-  <si>
-    <t>忍者面向下手持手里剑自然站立，循环动画</t>
-  </si>
-  <si>
-    <t>忍者扔出手里剑，一次性过渡动画</t>
-  </si>
-  <si>
-    <t>忍者持手里剑蓄力持续瞄准，准备扔出去，循环动画</t>
-  </si>
-  <si>
-    <t>忍者瞬移到不可落地的位置之后，掉下悬崖的动作，循环或一次性动画</t>
-  </si>
-  <si>
-    <t>忍者瞬移到可落地的位置之后，恢复动作到手持手里剑自然站立，一次性过渡动画</t>
-  </si>
-  <si>
-    <t>回旋镖被扔出瞬间，破空或地面溅起的烟尘等帧动画特效</t>
-  </si>
-  <si>
-    <t>回旋镖被扔出去时的状态，不需要自旋转，单帧或循环动画</t>
-  </si>
-  <si>
-    <t>忍者瞄准时的回旋镖状态，单帧或循环动画</t>
-  </si>
-  <si>
-    <t>回旋镖默认状态，Top Down 视角下的十字形回旋镖，单帧或循环动画</t>
-  </si>
-  <si>
-    <t>瞄准轨迹所用的点，单色像素点或小球体</t>
-  </si>
-  <si>
-    <t>回旋镖飞行时背后的轨迹粒子，单色像素点，或五像素十字即可，主要是确定颜色</t>
-  </si>
-  <si>
-    <t>人传送走的时候的帧动画特效</t>
-  </si>
-  <si>
-    <t>人传送到目的地时候的帧动画特效</t>
-  </si>
-  <si>
-    <t>建筑，屋顶是固定站立平台</t>
-  </si>
-  <si>
-    <t>飞行汽车，小型移动平台</t>
-  </si>
-  <si>
-    <t>飞空艇，大型移动平台</t>
-  </si>
-  <si>
-    <t>阻挡物，例如高塔、围栏等</t>
-  </si>
-  <si>
     <t>City_Background</t>
   </si>
   <si>
-    <t>TopDown 视角，城市背景</t>
-  </si>
-  <si>
     <t>Sprites</t>
   </si>
   <si>
@@ -233,22 +146,73 @@
     <t>High</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>_0X(Variants or Tiles)</t>
-  </si>
-  <si>
-    <t>Status (New/WIP/Done)</t>
-  </si>
-  <si>
     <t>Junce Wang</t>
   </si>
   <si>
     <t>First version</t>
+  </si>
+  <si>
+    <t>Status (New/WIP/Done/Outsourced)</t>
+  </si>
+  <si>
+    <t>Ninjia's idle pose, facing down.  Loop animation.</t>
+  </si>
+  <si>
+    <t>Ninjia hoding the Shyuriken and ready to throw it.  Single frame sprite.</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>Ninjia from aiming pose thorwing the Shyuriken and transit to idle pose.  Animation.</t>
+  </si>
+  <si>
+    <t>Ninjia falling from the ait to the abyss.  Single frame sprite.  (Mario-esh)</t>
+  </si>
+  <si>
+    <t>Ninjia activating teleporting ability.  Animation</t>
+  </si>
+  <si>
+    <t>Idle state of the boomerang.  Single frame or loop animation sprites.  No rotation.</t>
+  </si>
+  <si>
+    <t>Aiming state of boomerang.  Shining or emitting.  Single frame or loop animation sprites.</t>
+  </si>
+  <si>
+    <t>Thorwn state of boomerang.  Shining or emitting.  Single frame or loop animation sprites.</t>
+  </si>
+  <si>
+    <t>Trails behind the boomerang when moving.  Particle sprites.</t>
+  </si>
+  <si>
+    <t>Dust or air splash when thorwing the boomerang.  Animation sprites.</t>
+  </si>
+  <si>
+    <t>Aiming dot or indicator's particle unit.  Particle sprites.</t>
+  </si>
+  <si>
+    <t>VFX animation sprites when Ninjia teleports from somewhere.</t>
+  </si>
+  <si>
+    <t>VFX animation sprites when Ninjia teleports into somewhere.</t>
+  </si>
+  <si>
+    <t>Building floors.  Stationary platforms.</t>
+  </si>
+  <si>
+    <t>Flying cars, moving plarforms.</t>
+  </si>
+  <si>
+    <t>Air ship, larger moving plarfroms.</t>
+  </si>
+  <si>
+    <t>Obstacels.  Cylinders like towers or pipes.</t>
+  </si>
+  <si>
+    <t>Background of the city ground in top down view?</t>
+  </si>
+  <si>
+    <t>Simplified character assets and added English descriptions.</t>
   </si>
 </sst>
 </file>
@@ -305,8 +269,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70FAE4E7-6BF5-4AEA-A099-C53041F5BE13}" name="Table1" displayName="Table1" ref="A1:J1048576" totalsRowShown="0">
-  <autoFilter ref="A1:J1048576" xr:uid="{D3B59CEE-403F-4F96-AA2A-33461CD75439}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70FAE4E7-6BF5-4AEA-A099-C53041F5BE13}" name="Table1" displayName="Table1" ref="A1:J1048571" totalsRowShown="0">
+  <autoFilter ref="A1:J1048571" xr:uid="{D3B59CEE-403F-4F96-AA2A-33461CD75439}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{E6068E1E-B064-4715-AE12-CABE5356EFBD}" name="Category"/>
     <tableColumn id="2" xr3:uid="{63DA9891-2C33-4995-836D-9A8FA1F7A960}" name="Filename Prefix"/>
@@ -315,7 +279,7 @@
     <tableColumn id="5" xr3:uid="{32BF1732-9C2A-4901-833B-8E76A4E7D6AD}" name="Type"/>
     <tableColumn id="6" xr3:uid="{699763CA-B275-41CE-9A80-88EC9ACD32AA}" name="Description"/>
     <tableColumn id="7" xr3:uid="{E8799EC1-C2ED-4F9E-A6E4-ADF96D805A9D}" name="Priority"/>
-    <tableColumn id="8" xr3:uid="{9EE69AF0-1074-4079-AD29-C24B1EE70176}" name="Status (New/WIP/Done)"/>
+    <tableColumn id="8" xr3:uid="{9EE69AF0-1074-4079-AD29-C24B1EE70176}" name="Status (New/WIP/Done/Outsourced)"/>
     <tableColumn id="9" xr3:uid="{125D70D8-F238-408D-A46C-BD61935C5A69}" name="Date"/>
     <tableColumn id="10" xr3:uid="{AB5D9AF4-DF4B-420D-839A-A5213CEC001D}" name="Note"/>
   </tableColumns>
@@ -586,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE0BBFB-23A9-4186-8862-B079E0114A3E}">
-  <dimension ref="B2:D2"/>
+  <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,10 +567,21 @@
         <v>44437</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>44439</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -616,10 +591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +606,8 @@
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="81.85546875" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="10" max="10" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -639,13 +615,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -657,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -671,22 +647,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -694,22 +670,22 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -717,22 +693,22 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -740,22 +716,22 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -763,137 +739,137 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -901,22 +877,22 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -924,22 +900,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -947,252 +923,137 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" t="s">
-        <v>66</v>
-      </c>
-      <c r="G24" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>